<commit_message>
second morning routine done
</commit_message>
<xml_diff>
--- a/docs/logdata_general.xlsx
+++ b/docs/logdata_general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documents\GitHub\cern_data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8D73D9-FBDB-479C-80EB-4167EC89CF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF932B5B-E4B3-4880-BC28-F6690CB40EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F941097-CA86-4895-A431-AE92C65AA0EA}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
-  <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>V4 (V)</t>
   </si>
@@ -114,6 +108,36 @@
   </si>
   <si>
     <t>Redémarré</t>
+  </si>
+  <si>
+    <t>Pression externe (bar)</t>
+  </si>
+  <si>
+    <t>Mouvement -5</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Mouvement 5</t>
+  </si>
+  <si>
+    <t>Position affichée</t>
+  </si>
+  <si>
+    <t>Position physique</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>LN2 tube</t>
+  </si>
+  <si>
+    <t>Fichier-&gt;Marie</t>
+  </si>
+  <si>
+    <t>Envoyé</t>
   </si>
 </sst>
 </file>
@@ -153,15 +177,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED5233-F8B3-40D2-A4A6-FD6E6F7FFBE7}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,126 +510,159 @@
     <col min="3" max="3" width="11.109375" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" customWidth="1"/>
+    <col min="22" max="22" width="21.5546875" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" customWidth="1"/>
+    <col min="24" max="24" width="14.21875" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>45090</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0.44722222222222219</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <f>-193.96</f>
         <v>-193.96</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <f>-193.99</f>
         <v>-193.99</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>-194</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>-174.46</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>68.400000000000006</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>42.6</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>23.4</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>12.3</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>250</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>6</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="3">
         <v>16</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <v>90</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="P2">
+        <v>0.09</v>
+      </c>
+      <c r="Q2">
+        <v>0.08</v>
       </c>
       <c r="R2">
         <v>24</v>
@@ -616,60 +671,60 @@
         <v>24</v>
       </c>
       <c r="T2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B3" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
         <v>0.73749999999999993</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
         <v>-193.96</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>-193.99</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>-193.97</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>-193.99</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>47.5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>37.4</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>25.3</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>16.7</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>120</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>6</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <v>16</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>99</v>
       </c>
       <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="P3">
+        <v>0.09</v>
+      </c>
+      <c r="Q3">
+        <v>0.08</v>
       </c>
       <c r="R3">
         <v>24</v>
@@ -678,56 +733,146 @@
         <v>24</v>
       </c>
       <c r="T3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" t="s">
         <v>23</v>
       </c>
-      <c r="U3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
+      <c r="V3">
+        <v>163</v>
+      </c>
+      <c r="AC3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-193.86</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-193.89</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-193.84</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-144.12</v>
+      </c>
+      <c r="G4" s="3">
+        <v>65.7</v>
+      </c>
+      <c r="H4" s="3">
+        <v>44.2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>120</v>
+      </c>
+      <c r="L4" s="3">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3">
+        <v>16</v>
+      </c>
+      <c r="N4" s="3">
+        <v>95</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="R4">
+        <v>24</v>
+      </c>
+      <c r="S4">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4">
+        <v>150</v>
+      </c>
+      <c r="W4">
+        <v>595</v>
+      </c>
+      <c r="X4">
+        <v>608</v>
+      </c>
+      <c r="Y4">
+        <v>602</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA4">
+        <v>607</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>